<commit_message>
Event name as file name
</commit_message>
<xml_diff>
--- a/sheet3_2.xlsx
+++ b/sheet3_2.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t xml:space="preserve">Zjazd</t>
   </si>
@@ -109,13 +109,13 @@
     <t xml:space="preserve">Przedmiot 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Kajko</t>
+    <t xml:space="preserve">Kajko Słowianin</t>
   </si>
   <si>
     <t xml:space="preserve">Przedmiot 6</t>
   </si>
   <si>
-    <t xml:space="preserve">Kokosz</t>
+    <t xml:space="preserve">Kokosz Słowianin</t>
   </si>
   <si>
     <t xml:space="preserve">ZALICZENIA/EGZAMINY POPRAWKOWE</t>
@@ -551,7 +551,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -589,9 +589,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="n">
@@ -619,9 +617,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="8"/>
-      <c r="J2" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
@@ -723,9 +719,7 @@
         <v>13</v>
       </c>
       <c r="I6" s="27"/>
-      <c r="J6" s="22" t="n">
-        <v>2</v>
-      </c>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22"/>
@@ -865,9 +859,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="12"/>
-      <c r="J12" s="38" t="n">
-        <v>8</v>
-      </c>
+      <c r="J12" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -882,7 +874,7 @@
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1:D11" type="list">
-      <formula1>#NAZWA?</formula1>
+      <formula1>#nazwa?</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>